<commit_message>
"v1.0., First final version done"
</commit_message>
<xml_diff>
--- a/Process Dataframes/Efemerides.xlsx
+++ b/Process Dataframes/Efemerides.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="1203">
   <si>
     <t>Date</t>
   </si>
@@ -1482,6 +1482,9 @@
     <t>May 23</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1903</t>
+  </si>
+  <si>
     <t>Paris, France and Rome, Italy are connected by telephone for first time. Feel free to congratulate me for finding this picture at any time.</t>
   </si>
   <si>
@@ -1719,9 +1722,6 @@
     <t>June 16</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1903</t>
-  </si>
-  <si>
     <t>Henry Ford incorporates the Ford Motor Company with ten investors and $28,000. Ford will begin building automobiles on Mack Avenue in Detroit in a converted factory that previously produced wagons.</t>
   </si>
   <si>
@@ -2343,6 +2343,9 @@
     <t>August 17</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1982</t>
+  </si>
+  <si>
     <t>"The Visitors” by ABBA becomes the world’s first commercial music compact disc (CD) manufactured. Phillips and Sony co-developed the CD standard, which was designed to be the successor to the phonograph record.</t>
   </si>
   <si>
@@ -2659,9 +2662,6 @@
   </si>
   <si>
     <t>September 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1982</t>
   </si>
   <si>
     <t>Professor Scott Fahlman proposes the first known use of emoticons. The original message was retrieved from backup tape, which is displayed below.</t>
@@ -3678,7 +3678,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3686,6 +3686,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -3931,7 +3935,7 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3948,7 +3952,7 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3965,7 +3969,7 @@
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3982,7 +3986,7 @@
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3999,7 +4003,7 @@
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -4016,7 +4020,7 @@
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -4033,7 +4037,7 @@
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -4050,7 +4054,7 @@
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -4067,7 +4071,7 @@
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -4084,7 +4088,7 @@
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -4101,7 +4105,7 @@
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -4118,7 +4122,7 @@
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -4135,7 +4139,7 @@
       <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -4152,7 +4156,7 @@
       <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -4169,7 +4173,7 @@
       <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -4186,7 +4190,7 @@
       <c r="B17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -4203,7 +4207,7 @@
       <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -4220,7 +4224,7 @@
       <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -4237,7 +4241,7 @@
       <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -4254,7 +4258,7 @@
       <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -4271,7 +4275,7 @@
       <c r="B22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -4288,7 +4292,7 @@
       <c r="B23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -4305,7 +4309,7 @@
       <c r="B24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -4322,7 +4326,7 @@
       <c r="B25" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -4339,7 +4343,7 @@
       <c r="B26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -4356,7 +4360,7 @@
       <c r="B27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -4373,7 +4377,7 @@
       <c r="B28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -4390,7 +4394,7 @@
       <c r="B29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -4407,7 +4411,7 @@
       <c r="B30" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -4424,7 +4428,7 @@
       <c r="B31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -4441,7 +4445,7 @@
       <c r="B32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -4458,7 +4462,7 @@
       <c r="B33" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4475,7 +4479,7 @@
       <c r="B34" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -4492,7 +4496,7 @@
       <c r="B35" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4509,7 +4513,7 @@
       <c r="B36" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -4526,7 +4530,7 @@
       <c r="B37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -4543,7 +4547,7 @@
       <c r="B38" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -4560,7 +4564,7 @@
       <c r="B39" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4577,7 +4581,7 @@
       <c r="B40" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -4594,7 +4598,7 @@
       <c r="B41" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4611,7 +4615,7 @@
       <c r="B42" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -4628,7 +4632,7 @@
       <c r="B43" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -4645,7 +4649,7 @@
       <c r="B44" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -4662,7 +4666,7 @@
       <c r="B45" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4679,7 +4683,7 @@
       <c r="B46" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -4696,7 +4700,7 @@
       <c r="B47" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -4713,7 +4717,7 @@
       <c r="B48" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -4730,7 +4734,7 @@
       <c r="B49" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -4747,7 +4751,7 @@
       <c r="B50" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -4764,7 +4768,7 @@
       <c r="B51" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -4781,7 +4785,7 @@
       <c r="B52" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -4798,7 +4802,7 @@
       <c r="B53" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -4815,7 +4819,7 @@
       <c r="B54" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -4832,7 +4836,7 @@
       <c r="B55" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -4849,7 +4853,7 @@
       <c r="B56" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -4866,7 +4870,7 @@
       <c r="B57" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -4883,7 +4887,7 @@
       <c r="B58" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -4900,7 +4904,7 @@
       <c r="B59" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -4917,7 +4921,7 @@
       <c r="B60" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -4934,7 +4938,7 @@
       <c r="B61" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -4951,7 +4955,7 @@
       <c r="B62" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -4968,7 +4972,7 @@
       <c r="B63" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -4985,7 +4989,7 @@
       <c r="B64" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -5002,7 +5006,7 @@
       <c r="B65" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -5019,7 +5023,7 @@
       <c r="B66" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>222</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -5036,7 +5040,7 @@
       <c r="B67" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -5053,7 +5057,7 @@
       <c r="B68" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -5070,7 +5074,7 @@
       <c r="B69" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -5087,7 +5091,7 @@
       <c r="B70" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D70" s="2" t="s">
@@ -5104,7 +5108,7 @@
       <c r="B71" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -5121,7 +5125,7 @@
       <c r="B72" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -5138,7 +5142,7 @@
       <c r="B73" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>246</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -5155,7 +5159,7 @@
       <c r="B74" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="3" t="s">
         <v>250</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -5172,7 +5176,7 @@
       <c r="B75" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D75" s="2" t="s">
@@ -5189,7 +5193,7 @@
       <c r="B76" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -5206,7 +5210,7 @@
       <c r="B77" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D77" s="2" t="s">
@@ -5223,7 +5227,7 @@
       <c r="B78" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="3" t="s">
         <v>264</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -5240,7 +5244,7 @@
       <c r="B79" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -5257,7 +5261,7 @@
       <c r="B80" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -5274,7 +5278,7 @@
       <c r="B81" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>274</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -5291,7 +5295,7 @@
       <c r="B82" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>278</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -5308,7 +5312,7 @@
       <c r="B83" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -5325,7 +5329,7 @@
       <c r="B84" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -5342,7 +5346,7 @@
       <c r="B85" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -5359,7 +5363,7 @@
       <c r="B86" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -5376,7 +5380,7 @@
       <c r="B87" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="3" t="s">
         <v>294</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -5393,7 +5397,7 @@
       <c r="B88" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D88" s="2" t="s">
@@ -5410,7 +5414,7 @@
       <c r="B89" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -5427,7 +5431,7 @@
       <c r="B90" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="3" t="s">
         <v>304</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -5444,7 +5448,7 @@
       <c r="B91" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -5461,7 +5465,7 @@
       <c r="B92" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -5478,7 +5482,7 @@
       <c r="B93" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="3" t="s">
         <v>314</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -5495,7 +5499,7 @@
       <c r="B94" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="3" t="s">
         <v>318</v>
       </c>
       <c r="D94" s="2" t="s">
@@ -5512,7 +5516,7 @@
       <c r="B95" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -5529,7 +5533,7 @@
       <c r="B96" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="3" t="s">
         <v>325</v>
       </c>
       <c r="D96" s="2" t="s">
@@ -5546,7 +5550,7 @@
       <c r="B97" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>329</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -5563,7 +5567,7 @@
       <c r="B98" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="3" t="s">
         <v>333</v>
       </c>
       <c r="D98" s="2" t="s">
@@ -5580,7 +5584,7 @@
       <c r="B99" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -5597,7 +5601,7 @@
       <c r="B100" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="3" t="s">
         <v>340</v>
       </c>
       <c r="D100" s="2" t="s">
@@ -5614,7 +5618,7 @@
       <c r="B101" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="3" t="s">
         <v>344</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -5631,7 +5635,7 @@
       <c r="B102" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D102" s="2" t="s">
@@ -5648,7 +5652,7 @@
       <c r="B103" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -5665,7 +5669,7 @@
       <c r="B104" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="2" t="s">
@@ -5682,7 +5686,7 @@
       <c r="B105" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -5699,7 +5703,7 @@
       <c r="B106" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D106" s="2" t="s">
@@ -5716,7 +5720,7 @@
       <c r="B107" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -5733,7 +5737,7 @@
       <c r="B108" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="3" t="s">
         <v>367</v>
       </c>
       <c r="D108" s="2" t="s">
@@ -5750,7 +5754,7 @@
       <c r="B109" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -5767,7 +5771,7 @@
       <c r="B110" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="3" t="s">
         <v>374</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -5784,7 +5788,7 @@
       <c r="B111" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -5801,7 +5805,7 @@
       <c r="B112" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -5818,7 +5822,7 @@
       <c r="B113" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>384</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -5835,7 +5839,7 @@
       <c r="B114" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="3" t="s">
         <v>388</v>
       </c>
       <c r="D114" s="2" t="s">
@@ -5852,7 +5856,7 @@
       <c r="B115" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -5869,7 +5873,7 @@
       <c r="B116" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D116" s="2" t="s">
@@ -5886,7 +5890,7 @@
       <c r="B117" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -5903,7 +5907,7 @@
       <c r="B118" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D118" s="2" t="s">
@@ -5920,7 +5924,7 @@
       <c r="B119" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -5937,7 +5941,7 @@
       <c r="B120" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -5954,7 +5958,7 @@
       <c r="B121" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -5971,7 +5975,7 @@
       <c r="B122" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D122" s="2" t="s">
@@ -5988,7 +5992,7 @@
       <c r="B123" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -6005,7 +6009,7 @@
       <c r="B124" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D124" s="2" t="s">
@@ -6022,8 +6026,8 @@
       <c r="B125" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C125" s="2">
-        <v>2000.0</v>
+      <c r="C125" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>423</v>
@@ -6039,7 +6043,7 @@
       <c r="B126" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="3" t="s">
         <v>222</v>
       </c>
       <c r="D126" s="2" t="s">
@@ -6056,7 +6060,7 @@
       <c r="B127" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D127" s="2" t="s">
@@ -6073,7 +6077,7 @@
       <c r="B128" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="3" t="s">
         <v>432</v>
       </c>
       <c r="D128" s="2" t="s">
@@ -6090,7 +6094,7 @@
       <c r="B129" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="3" t="s">
         <v>436</v>
       </c>
       <c r="D129" s="2" t="s">
@@ -6107,7 +6111,7 @@
       <c r="B130" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D130" s="2" t="s">
@@ -6124,7 +6128,7 @@
       <c r="B131" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="3" t="s">
         <v>443</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -6141,7 +6145,7 @@
       <c r="B132" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D132" s="2" t="s">
@@ -6158,7 +6162,7 @@
       <c r="B133" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="3" t="s">
         <v>451</v>
       </c>
       <c r="D133" s="2" t="s">
@@ -6175,7 +6179,7 @@
       <c r="B134" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D134" s="2" t="s">
@@ -6192,7 +6196,7 @@
       <c r="B135" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="3" t="s">
         <v>318</v>
       </c>
       <c r="D135" s="2" t="s">
@@ -6209,7 +6213,7 @@
       <c r="B136" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D136" s="2" t="s">
@@ -6226,7 +6230,7 @@
       <c r="B137" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="3" t="s">
         <v>464</v>
       </c>
       <c r="D137" s="2" t="s">
@@ -6243,7 +6247,7 @@
       <c r="B138" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D138" s="2" t="s">
@@ -6260,7 +6264,7 @@
       <c r="B139" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -6277,7 +6281,7 @@
       <c r="B140" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D140" s="2" t="s">
@@ -6294,7 +6298,7 @@
       <c r="B141" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="3" t="s">
         <v>477</v>
       </c>
       <c r="D141" s="2" t="s">
@@ -6311,7 +6315,7 @@
       <c r="B142" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D142" s="2" t="s">
@@ -6328,8 +6332,8 @@
       <c r="B143" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C143" s="3">
-        <v>1980.0</v>
+      <c r="C143" s="4" t="s">
+        <v>481</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>485</v>
@@ -6345,14 +6349,14 @@
       <c r="B144" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="C144" s="3">
-        <v>1903.0</v>
+      <c r="C144" s="4" t="s">
+        <v>488</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
@@ -6360,16 +6364,16 @@
         <v>143.0</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="C145" s="2" t="s">
         <v>491</v>
       </c>
+      <c r="C145" s="3" t="s">
+        <v>492</v>
+      </c>
       <c r="D145" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
@@ -6377,16 +6381,16 @@
         <v>144.0</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="C146" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
@@ -6394,16 +6398,16 @@
         <v>145.0</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C147" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1">
@@ -6411,16 +6415,16 @@
         <v>146.0</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="C148" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1">
@@ -6428,16 +6432,16 @@
         <v>147.0</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C149" s="2" t="s">
         <v>504</v>
       </c>
+      <c r="C149" s="3" t="s">
+        <v>505</v>
+      </c>
       <c r="D149" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1">
@@ -6445,16 +6449,16 @@
         <v>148.0</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="C150" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="151" ht="15.75" customHeight="1">
@@ -6462,16 +6466,16 @@
         <v>149.0</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C151" s="2" t="s">
         <v>511</v>
       </c>
+      <c r="C151" s="3" t="s">
+        <v>512</v>
+      </c>
       <c r="D151" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="152" ht="15.75" customHeight="1">
@@ -6479,16 +6483,16 @@
         <v>150.0</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="C152" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
@@ -6496,16 +6500,16 @@
         <v>151.0</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="C153" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="154" ht="15.75" customHeight="1">
@@ -6513,16 +6517,16 @@
         <v>152.0</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="C154" s="2" t="s">
         <v>521</v>
       </c>
+      <c r="C154" s="3" t="s">
+        <v>522</v>
+      </c>
       <c r="D154" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="155" ht="15.75" customHeight="1">
@@ -6530,16 +6534,16 @@
         <v>153.0</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="C155" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C155" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="156" ht="15.75" customHeight="1">
@@ -6547,16 +6551,16 @@
         <v>154.0</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="C156" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="157" ht="15.75" customHeight="1">
@@ -6564,16 +6568,16 @@
         <v>155.0</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="C157" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C157" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1">
@@ -6581,33 +6585,33 @@
         <v>156.0</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="C158" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="1">
         <v>157.0</v>
       </c>
-      <c r="B159" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C159" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="D159" s="3" t="s">
+      <c r="B159" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="C159" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D159" s="5" t="s">
         <v>538</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="160" ht="15.75" customHeight="1">
@@ -6615,16 +6619,16 @@
         <v>158.0</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="C160" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="C160" s="3" t="s">
+        <v>541</v>
+      </c>
       <c r="D160" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="161" ht="15.75" customHeight="1">
@@ -6632,16 +6636,16 @@
         <v>159.0</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="C161" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="162" ht="15.75" customHeight="1">
@@ -6649,16 +6653,16 @@
         <v>160.0</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C162" s="2" t="s">
         <v>547</v>
       </c>
+      <c r="C162" s="3" t="s">
+        <v>548</v>
+      </c>
       <c r="D162" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
@@ -6666,33 +6670,33 @@
         <v>161.0</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>540</v>
+        <v>551</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>541</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="1">
         <v>162.0</v>
       </c>
-      <c r="B164" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="C164" s="3">
-        <v>1967.0</v>
-      </c>
-      <c r="D164" s="3" t="s">
+      <c r="B164" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="C164" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D164" s="5" t="s">
         <v>555</v>
+      </c>
+      <c r="E164" s="5" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
@@ -6700,16 +6704,16 @@
         <v>163.0</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="C165" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1">
@@ -6717,16 +6721,16 @@
         <v>164.0</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C166" s="2" t="s">
         <v>560</v>
       </c>
+      <c r="C166" s="3" t="s">
+        <v>561</v>
+      </c>
       <c r="D166" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1">
@@ -6734,16 +6738,16 @@
         <v>165.0</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="C167" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1">
@@ -6751,10 +6755,10 @@
         <v>166.0</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C168" s="2" t="s">
         <v>567</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>488</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>568</v>
@@ -6770,7 +6774,7 @@
       <c r="B169" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D169" s="2" t="s">
@@ -6787,7 +6791,7 @@
       <c r="B170" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D170" s="2" t="s">
@@ -6804,7 +6808,7 @@
       <c r="B171" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="3" t="s">
         <v>294</v>
       </c>
       <c r="D171" s="2" t="s">
@@ -6821,7 +6825,7 @@
       <c r="B172" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="3" t="s">
         <v>580</v>
       </c>
       <c r="D172" s="2" t="s">
@@ -6835,16 +6839,16 @@
       <c r="A173" s="1">
         <v>171.0</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B173" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="C173" s="3">
-        <v>2004.0</v>
-      </c>
-      <c r="D173" s="3" t="s">
+      <c r="C173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D173" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="E173" s="3" t="s">
+      <c r="E173" s="5" t="s">
         <v>585</v>
       </c>
     </row>
@@ -6855,7 +6859,7 @@
       <c r="B174" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C174" s="3" t="s">
         <v>587</v>
       </c>
       <c r="D174" s="2" t="s">
@@ -6872,7 +6876,7 @@
       <c r="B175" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="3" t="s">
         <v>591</v>
       </c>
       <c r="D175" s="2" t="s">
@@ -6889,7 +6893,7 @@
       <c r="B176" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C176" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D176" s="2" t="s">
@@ -6906,7 +6910,7 @@
       <c r="B177" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D177" s="2" t="s">
@@ -6923,7 +6927,7 @@
       <c r="B178" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="3" t="s">
         <v>601</v>
       </c>
       <c r="D178" s="2" t="s">
@@ -6940,7 +6944,7 @@
       <c r="B179" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="C179" s="3" t="s">
         <v>605</v>
       </c>
       <c r="D179" s="2" t="s">
@@ -6957,7 +6961,7 @@
       <c r="B180" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C180" s="3" t="s">
         <v>374</v>
       </c>
       <c r="D180" s="2" t="s">
@@ -6974,7 +6978,7 @@
       <c r="B181" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C181" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D181" s="2" t="s">
@@ -6991,7 +6995,7 @@
       <c r="B182" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="3" t="s">
         <v>615</v>
       </c>
       <c r="D182" s="2" t="s">
@@ -7008,7 +7012,7 @@
       <c r="B183" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="C183" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D183" s="2" t="s">
@@ -7025,7 +7029,7 @@
       <c r="B184" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" s="3" t="s">
         <v>622</v>
       </c>
       <c r="D184" s="2" t="s">
@@ -7042,7 +7046,7 @@
       <c r="B185" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D185" s="2" t="s">
@@ -7059,7 +7063,7 @@
       <c r="B186" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C186" s="3" t="s">
         <v>630</v>
       </c>
       <c r="D186" s="2" t="s">
@@ -7076,7 +7080,7 @@
       <c r="B187" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C187" s="3" t="s">
         <v>634</v>
       </c>
       <c r="D187" s="2" t="s">
@@ -7093,7 +7097,7 @@
       <c r="B188" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C188" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D188" s="2" t="s">
@@ -7110,7 +7114,7 @@
       <c r="B189" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="3" t="s">
         <v>641</v>
       </c>
       <c r="D189" s="2" t="s">
@@ -7127,7 +7131,7 @@
       <c r="B190" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="3" t="s">
         <v>645</v>
       </c>
       <c r="D190" s="2" t="s">
@@ -7144,7 +7148,7 @@
       <c r="B191" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D191" s="2" t="s">
@@ -7161,7 +7165,7 @@
       <c r="B192" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C192" s="3" t="s">
         <v>652</v>
       </c>
       <c r="D192" s="2" t="s">
@@ -7178,7 +7182,7 @@
       <c r="B193" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C193" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D193" s="2" t="s">
@@ -7195,7 +7199,7 @@
       <c r="B194" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C194" s="3" t="s">
         <v>659</v>
       </c>
       <c r="D194" s="2" t="s">
@@ -7212,7 +7216,7 @@
       <c r="B195" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C195" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D195" s="2" t="s">
@@ -7226,16 +7230,16 @@
       <c r="A196" s="1">
         <v>194.0</v>
       </c>
-      <c r="B196" s="3" t="s">
+      <c r="B196" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="C196" s="3">
-        <v>1965.0</v>
-      </c>
-      <c r="D196" s="3" t="s">
+      <c r="C196" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D196" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="E196" s="3" t="s">
+      <c r="E196" s="5" t="s">
         <v>667</v>
       </c>
     </row>
@@ -7246,7 +7250,7 @@
       <c r="B197" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C197" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D197" s="2" t="s">
@@ -7263,7 +7267,7 @@
       <c r="B198" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="C198" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D198" s="2" t="s">
@@ -7280,7 +7284,7 @@
       <c r="B199" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C199" s="3" t="s">
         <v>675</v>
       </c>
       <c r="D199" s="2" t="s">
@@ -7297,7 +7301,7 @@
       <c r="B200" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C200" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D200" s="2" t="s">
@@ -7314,7 +7318,7 @@
       <c r="B201" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D201" s="2" t="s">
@@ -7331,7 +7335,7 @@
       <c r="B202" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D202" s="2" t="s">
@@ -7348,7 +7352,7 @@
       <c r="B203" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C203" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D203" s="2" t="s">
@@ -7365,7 +7369,7 @@
       <c r="B204" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="C204" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D204" s="2" t="s">
@@ -7382,7 +7386,7 @@
       <c r="B205" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="C205" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D205" s="2" t="s">
@@ -7399,7 +7403,7 @@
       <c r="B206" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="C206" s="3" t="s">
         <v>580</v>
       </c>
       <c r="D206" s="2" t="s">
@@ -7416,7 +7420,7 @@
       <c r="B207" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="C207" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D207" s="2" t="s">
@@ -7433,7 +7437,7 @@
       <c r="B208" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="C208" s="2" t="s">
+      <c r="C208" s="3" t="s">
         <v>703</v>
       </c>
       <c r="D208" s="2" t="s">
@@ -7450,7 +7454,7 @@
       <c r="B209" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="C209" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D209" s="2" t="s">
@@ -7467,7 +7471,7 @@
       <c r="B210" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="C210" s="2" t="s">
+      <c r="C210" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D210" s="2" t="s">
@@ -7484,13 +7488,13 @@
       <c r="B211" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="C211" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="D211" s="3" t="s">
+      <c r="D211" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="E211" s="3" t="s">
+      <c r="E211" s="5" t="s">
         <v>715</v>
       </c>
     </row>
@@ -7498,16 +7502,16 @@
       <c r="A212" s="1">
         <v>210.0</v>
       </c>
-      <c r="B212" s="3" t="s">
+      <c r="B212" s="5" t="s">
         <v>716</v>
       </c>
-      <c r="C212" s="3">
-        <v>1979.0</v>
-      </c>
-      <c r="D212" s="3" t="s">
+      <c r="C212" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="D212" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="E212" s="3" t="s">
+      <c r="E212" s="5" t="s">
         <v>718</v>
       </c>
     </row>
@@ -7518,7 +7522,7 @@
       <c r="B213" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="C213" s="3" t="s">
         <v>720</v>
       </c>
       <c r="D213" s="2" t="s">
@@ -7535,7 +7539,7 @@
       <c r="B214" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="C214" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D214" s="2" t="s">
@@ -7552,7 +7556,7 @@
       <c r="B215" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="C215" s="3" t="s">
         <v>727</v>
       </c>
       <c r="D215" s="2" t="s">
@@ -7569,7 +7573,7 @@
       <c r="B216" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="C216" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D216" s="2" t="s">
@@ -7586,7 +7590,7 @@
       <c r="B217" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="C217" s="2" t="s">
+      <c r="C217" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D217" s="2" t="s">
@@ -7603,8 +7607,8 @@
       <c r="B218" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="C218" s="2" t="s">
-        <v>547</v>
+      <c r="C218" s="3" t="s">
+        <v>548</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>737</v>
@@ -7620,7 +7624,7 @@
       <c r="B219" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C219" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D219" s="2" t="s">
@@ -7637,7 +7641,7 @@
       <c r="B220" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="C220" s="3" t="s">
         <v>743</v>
       </c>
       <c r="D220" s="2" t="s">
@@ -7654,7 +7658,7 @@
       <c r="B221" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="C221" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D221" s="2" t="s">
@@ -7671,7 +7675,7 @@
       <c r="B222" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D222" s="2" t="s">
@@ -7688,8 +7692,8 @@
       <c r="B223" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C223" s="2" t="s">
-        <v>521</v>
+      <c r="C223" s="3" t="s">
+        <v>522</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>753</v>
@@ -7705,7 +7709,7 @@
       <c r="B224" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D224" s="2" t="s">
@@ -7722,7 +7726,7 @@
       <c r="B225" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="C225" s="2" t="s">
+      <c r="C225" s="3" t="s">
         <v>759</v>
       </c>
       <c r="D225" s="2" t="s">
@@ -7739,7 +7743,7 @@
       <c r="B226" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D226" s="2" t="s">
@@ -7756,7 +7760,7 @@
       <c r="B227" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="C227" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D227" s="2" t="s">
@@ -7773,7 +7777,7 @@
       <c r="B228" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C228" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D228" s="2" t="s">
@@ -7790,7 +7794,7 @@
       <c r="B229" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="C229" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D229" s="2" t="s">
@@ -7804,17 +7808,17 @@
       <c r="A230" s="1">
         <v>228.0</v>
       </c>
-      <c r="B230" s="3" t="s">
+      <c r="B230" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="C230" s="3">
-        <v>1982.0</v>
-      </c>
-      <c r="D230" s="3" t="s">
+      <c r="C230" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="E230" s="3" t="s">
+      <c r="D230" s="5" t="s">
         <v>776</v>
+      </c>
+      <c r="E230" s="5" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
@@ -7822,16 +7826,16 @@
         <v>229.0</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="C231" s="2" t="s">
         <v>778</v>
       </c>
+      <c r="C231" s="3" t="s">
+        <v>779</v>
+      </c>
       <c r="D231" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1">
@@ -7839,16 +7843,16 @@
         <v>230.0</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="C232" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C232" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1">
@@ -7856,16 +7860,16 @@
         <v>231.0</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>784</v>
-      </c>
-      <c r="C233" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="C233" s="3" t="s">
+        <v>786</v>
+      </c>
       <c r="D233" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="234" ht="15.75" customHeight="1">
@@ -7873,16 +7877,16 @@
         <v>232.0</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="C234" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C234" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1">
@@ -7890,16 +7894,16 @@
         <v>233.0</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>504</v>
+        <v>792</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>505</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1">
@@ -7907,16 +7911,16 @@
         <v>234.0</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>794</v>
-      </c>
-      <c r="C236" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="C236" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
@@ -7924,16 +7928,16 @@
         <v>235.0</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>797</v>
-      </c>
-      <c r="C237" s="2" t="s">
         <v>798</v>
       </c>
+      <c r="C237" s="3" t="s">
+        <v>799</v>
+      </c>
       <c r="D237" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
@@ -7941,16 +7945,16 @@
         <v>236.0</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>801</v>
-      </c>
-      <c r="C238" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="C238" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
@@ -7958,16 +7962,16 @@
         <v>237.0</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>804</v>
-      </c>
-      <c r="C239" s="2" t="s">
         <v>805</v>
       </c>
+      <c r="C239" s="3" t="s">
+        <v>806</v>
+      </c>
       <c r="D239" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
@@ -7975,16 +7979,16 @@
         <v>238.0</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>808</v>
-      </c>
-      <c r="C240" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="C240" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1">
@@ -7992,16 +7996,16 @@
         <v>239.0</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="C241" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="C241" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1">
@@ -8009,16 +8013,16 @@
         <v>240.0</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="C242" s="2" t="s">
         <v>815</v>
       </c>
+      <c r="C242" s="3" t="s">
+        <v>816</v>
+      </c>
       <c r="D242" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
@@ -8026,16 +8030,16 @@
         <v>241.0</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>818</v>
-      </c>
-      <c r="C243" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="C243" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
@@ -8043,16 +8047,16 @@
         <v>242.0</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="C244" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="C244" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E244" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
@@ -8060,16 +8064,16 @@
         <v>243.0</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="C245" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="C245" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
@@ -8077,16 +8081,16 @@
         <v>244.0</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>827</v>
-      </c>
-      <c r="C246" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C246" s="3" t="s">
         <v>410</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1">
@@ -8094,16 +8098,16 @@
         <v>245.0</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="C247" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C247" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1">
@@ -8111,16 +8115,16 @@
         <v>246.0</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>833</v>
-      </c>
-      <c r="C248" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C248" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
@@ -8128,16 +8132,16 @@
         <v>247.0</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>836</v>
-      </c>
-      <c r="C249" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="C249" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1">
@@ -8145,16 +8149,16 @@
         <v>248.0</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="C250" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C250" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E250" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1">
@@ -8162,16 +8166,16 @@
         <v>249.0</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C251" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="C251" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1">
@@ -8179,16 +8183,16 @@
         <v>250.0</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C252" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="C252" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
@@ -8196,16 +8200,16 @@
         <v>251.0</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>848</v>
-      </c>
-      <c r="C253" s="2" t="s">
         <v>849</v>
       </c>
+      <c r="C253" s="3" t="s">
+        <v>850</v>
+      </c>
       <c r="D253" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
@@ -8213,16 +8217,16 @@
         <v>252.0</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C254" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C254" s="3" t="s">
         <v>659</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
@@ -8230,16 +8234,16 @@
         <v>253.0</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="C255" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C255" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E255" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
@@ -8247,16 +8251,16 @@
         <v>254.0</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="C256" s="2" t="s">
         <v>859</v>
       </c>
+      <c r="C256" s="3" t="s">
+        <v>860</v>
+      </c>
       <c r="D256" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1">
@@ -8264,16 +8268,16 @@
         <v>255.0</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="C257" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C257" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="258" ht="15.75" customHeight="1">
@@ -8281,16 +8285,16 @@
         <v>256.0</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="C258" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C258" s="3" t="s">
         <v>340</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="259" ht="15.75" customHeight="1">
@@ -8298,16 +8302,16 @@
         <v>257.0</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>868</v>
-      </c>
-      <c r="C259" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="C259" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="260" ht="15.75" customHeight="1">
@@ -8315,16 +8319,16 @@
         <v>258.0</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>871</v>
-      </c>
-      <c r="C260" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C260" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="261" ht="15.75" customHeight="1">
@@ -8332,16 +8336,16 @@
         <v>259.0</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>874</v>
-      </c>
-      <c r="C261" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="C261" s="3" t="s">
         <v>294</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E261" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="262" ht="15.75" customHeight="1">
@@ -8349,16 +8353,16 @@
         <v>260.0</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="C262" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="C262" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="263" ht="15.75" customHeight="1">
@@ -8366,10 +8370,10 @@
         <v>261.0</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>880</v>
-      </c>
-      <c r="C263" s="2" t="s">
         <v>881</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>775</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>882</v>
@@ -8385,7 +8389,7 @@
       <c r="B264" s="2" t="s">
         <v>884</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C264" s="3" t="s">
         <v>432</v>
       </c>
       <c r="D264" s="2" t="s">
@@ -8402,7 +8406,7 @@
       <c r="B265" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C265" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D265" s="2" t="s">
@@ -8419,7 +8423,7 @@
       <c r="B266" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="C266" s="2" t="s">
+      <c r="C266" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D266" s="2" t="s">
@@ -8436,7 +8440,7 @@
       <c r="B267" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="C267" s="2" t="s">
+      <c r="C267" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D267" s="2" t="s">
@@ -8453,7 +8457,7 @@
       <c r="B268" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="C268" s="2" t="s">
+      <c r="C268" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D268" s="2" t="s">
@@ -8470,7 +8474,7 @@
       <c r="B269" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="C269" s="2" t="s">
+      <c r="C269" s="3" t="s">
         <v>318</v>
       </c>
       <c r="D269" s="2" t="s">
@@ -8487,7 +8491,7 @@
       <c r="B270" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="C270" s="2" t="s">
+      <c r="C270" s="3" t="s">
         <v>318</v>
       </c>
       <c r="D270" s="2" t="s">
@@ -8501,10 +8505,10 @@
       <c r="A271" s="1">
         <v>269.0</v>
       </c>
-      <c r="B271" s="3" t="s">
+      <c r="B271" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C271" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D271" s="2" t="s">
@@ -8521,7 +8525,7 @@
       <c r="B272" s="2" t="s">
         <v>908</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="C272" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D272" s="2" t="s">
@@ -8538,7 +8542,7 @@
       <c r="B273" s="2" t="s">
         <v>911</v>
       </c>
-      <c r="C273" s="2" t="s">
+      <c r="C273" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D273" s="2" t="s">
@@ -8555,7 +8559,7 @@
       <c r="B274" s="2" t="s">
         <v>914</v>
       </c>
-      <c r="C274" s="2" t="s">
+      <c r="C274" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D274" s="2" t="s">
@@ -8572,8 +8576,8 @@
       <c r="B275" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="C275" s="2" t="s">
-        <v>881</v>
+      <c r="C275" s="3" t="s">
+        <v>775</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>918</v>
@@ -8589,7 +8593,7 @@
       <c r="B276" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="C276" s="2" t="s">
+      <c r="C276" s="3" t="s">
         <v>250</v>
       </c>
       <c r="D276" s="2" t="s">
@@ -8606,7 +8610,7 @@
       <c r="B277" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="C277" s="2" t="s">
+      <c r="C277" s="3" t="s">
         <v>580</v>
       </c>
       <c r="D277" s="2" t="s">
@@ -8623,7 +8627,7 @@
       <c r="B278" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="C278" s="2" t="s">
+      <c r="C278" s="3" t="s">
         <v>645</v>
       </c>
       <c r="D278" s="2" t="s">
@@ -8640,8 +8644,8 @@
       <c r="B279" s="2" t="s">
         <v>929</v>
       </c>
-      <c r="C279" s="2" t="s">
-        <v>798</v>
+      <c r="C279" s="3" t="s">
+        <v>799</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>930</v>
@@ -8657,7 +8661,7 @@
       <c r="B280" s="2" t="s">
         <v>932</v>
       </c>
-      <c r="C280" s="2" t="s">
+      <c r="C280" s="3" t="s">
         <v>933</v>
       </c>
       <c r="D280" s="2" t="s">
@@ -8674,7 +8678,7 @@
       <c r="B281" s="2" t="s">
         <v>936</v>
       </c>
-      <c r="C281" s="2" t="s">
+      <c r="C281" s="3" t="s">
         <v>432</v>
       </c>
       <c r="D281" s="2" t="s">
@@ -8691,7 +8695,7 @@
       <c r="B282" s="2" t="s">
         <v>939</v>
       </c>
-      <c r="C282" s="2" t="s">
+      <c r="C282" s="3" t="s">
         <v>222</v>
       </c>
       <c r="D282" s="2" t="s">
@@ -8708,7 +8712,7 @@
       <c r="B283" s="2" t="s">
         <v>942</v>
       </c>
-      <c r="C283" s="2" t="s">
+      <c r="C283" s="3" t="s">
         <v>226</v>
       </c>
       <c r="D283" s="2" t="s">
@@ -8725,7 +8729,7 @@
       <c r="B284" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="C284" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D284" s="2" t="s">
@@ -8742,8 +8746,8 @@
       <c r="B285" s="2" t="s">
         <v>948</v>
       </c>
-      <c r="C285" s="2" t="s">
-        <v>859</v>
+      <c r="C285" s="3" t="s">
+        <v>860</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>949</v>
@@ -8759,7 +8763,7 @@
       <c r="B286" s="2" t="s">
         <v>951</v>
       </c>
-      <c r="C286" s="2" t="s">
+      <c r="C286" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D286" s="2" t="s">
@@ -8776,7 +8780,7 @@
       <c r="B287" s="2" t="s">
         <v>954</v>
       </c>
-      <c r="C287" s="2" t="s">
+      <c r="C287" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D287" s="2" t="s">
@@ -8793,7 +8797,7 @@
       <c r="B288" s="2" t="s">
         <v>957</v>
       </c>
-      <c r="C288" s="2" t="s">
+      <c r="C288" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D288" s="2" t="s">
@@ -8810,7 +8814,7 @@
       <c r="B289" s="2" t="s">
         <v>960</v>
       </c>
-      <c r="C289" s="2" t="s">
+      <c r="C289" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D289" s="2" t="s">
@@ -8827,7 +8831,7 @@
       <c r="B290" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="C290" s="3" t="s">
         <v>340</v>
       </c>
       <c r="D290" s="2" t="s">
@@ -8844,7 +8848,7 @@
       <c r="B291" s="2" t="s">
         <v>966</v>
       </c>
-      <c r="C291" s="2" t="s">
+      <c r="C291" s="3" t="s">
         <v>659</v>
       </c>
       <c r="D291" s="2" t="s">
@@ -8861,7 +8865,7 @@
       <c r="B292" s="2" t="s">
         <v>969</v>
       </c>
-      <c r="C292" s="2" t="s">
+      <c r="C292" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D292" s="2" t="s">
@@ -8878,7 +8882,7 @@
       <c r="B293" s="2" t="s">
         <v>972</v>
       </c>
-      <c r="C293" s="2" t="s">
+      <c r="C293" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D293" s="2" t="s">
@@ -8895,7 +8899,7 @@
       <c r="B294" s="2" t="s">
         <v>975</v>
       </c>
-      <c r="C294" s="2" t="s">
+      <c r="C294" s="3" t="s">
         <v>976</v>
       </c>
       <c r="D294" s="2" t="s">
@@ -8912,7 +8916,7 @@
       <c r="B295" s="2" t="s">
         <v>979</v>
       </c>
-      <c r="C295" s="2" t="s">
+      <c r="C295" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D295" s="2" t="s">
@@ -8929,8 +8933,8 @@
       <c r="B296" s="2" t="s">
         <v>982</v>
       </c>
-      <c r="C296" s="2" t="s">
-        <v>805</v>
+      <c r="C296" s="3" t="s">
+        <v>806</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>983</v>
@@ -8946,7 +8950,7 @@
       <c r="B297" s="2" t="s">
         <v>985</v>
       </c>
-      <c r="C297" s="2" t="s">
+      <c r="C297" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D297" s="2" t="s">
@@ -8963,7 +8967,7 @@
       <c r="B298" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="C298" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D298" s="2" t="s">
@@ -8980,7 +8984,7 @@
       <c r="B299" s="2" t="s">
         <v>991</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="C299" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D299" s="2" t="s">
@@ -8997,7 +9001,7 @@
       <c r="B300" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="C300" s="3" t="s">
         <v>995</v>
       </c>
       <c r="D300" s="2" t="s">
@@ -9011,16 +9015,16 @@
       <c r="A301" s="1">
         <v>299.0</v>
       </c>
-      <c r="B301" s="3" t="s">
+      <c r="B301" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="C301" s="3">
-        <v>1980.0</v>
-      </c>
-      <c r="D301" s="3" t="s">
+      <c r="C301" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="D301" s="5" t="s">
         <v>999</v>
       </c>
-      <c r="E301" s="3" t="s">
+      <c r="E301" s="5" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -9031,7 +9035,7 @@
       <c r="B302" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="C302" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D302" s="2" t="s">
@@ -9045,16 +9049,16 @@
       <c r="A303" s="1">
         <v>301.0</v>
       </c>
-      <c r="B303" s="3" t="s">
+      <c r="B303" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="C303" s="3">
-        <v>1969.0</v>
-      </c>
-      <c r="D303" s="3" t="s">
+      <c r="C303" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="D303" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="E303" s="3" t="s">
+      <c r="E303" s="5" t="s">
         <v>1006</v>
       </c>
     </row>
@@ -9065,13 +9069,13 @@
       <c r="B304" s="2" t="s">
         <v>1007</v>
       </c>
-      <c r="C304" s="2" t="s">
-        <v>805</v>
-      </c>
-      <c r="D304" s="3" t="s">
+      <c r="C304" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="D304" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="E304" s="3" t="s">
+      <c r="E304" s="5" t="s">
         <v>1009</v>
       </c>
     </row>
@@ -9082,7 +9086,7 @@
       <c r="B305" s="2" t="s">
         <v>1010</v>
       </c>
-      <c r="C305" s="2" t="s">
+      <c r="C305" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D305" s="2" t="s">
@@ -9099,7 +9103,7 @@
       <c r="B306" s="2" t="s">
         <v>1013</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="C306" s="3" t="s">
         <v>432</v>
       </c>
       <c r="D306" s="2" t="s">
@@ -9116,7 +9120,7 @@
       <c r="B307" s="2" t="s">
         <v>1016</v>
       </c>
-      <c r="C307" s="2" t="s">
+      <c r="C307" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D307" s="2" t="s">
@@ -9133,7 +9137,7 @@
       <c r="B308" s="2" t="s">
         <v>1019</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="C308" s="3" t="s">
         <v>645</v>
       </c>
       <c r="D308" s="2" t="s">
@@ -9150,8 +9154,8 @@
       <c r="B309" s="2" t="s">
         <v>1022</v>
       </c>
-      <c r="C309" s="2" t="s">
-        <v>881</v>
+      <c r="C309" s="3" t="s">
+        <v>775</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>1023</v>
@@ -9167,7 +9171,7 @@
       <c r="B310" s="2" t="s">
         <v>1025</v>
       </c>
-      <c r="C310" s="2" t="s">
+      <c r="C310" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D310" s="2" t="s">
@@ -9184,7 +9188,7 @@
       <c r="B311" s="2" t="s">
         <v>1028</v>
       </c>
-      <c r="C311" s="2" t="s">
+      <c r="C311" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D311" s="2" t="s">
@@ -9201,7 +9205,7 @@
       <c r="B312" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="C312" s="2" t="s">
+      <c r="C312" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D312" s="2" t="s">
@@ -9218,7 +9222,7 @@
       <c r="B313" s="2" t="s">
         <v>1034</v>
       </c>
-      <c r="C313" s="2" t="s">
+      <c r="C313" s="3" t="s">
         <v>1035</v>
       </c>
       <c r="D313" s="2" t="s">
@@ -9232,16 +9236,16 @@
       <c r="A314" s="1">
         <v>312.0</v>
       </c>
-      <c r="B314" s="3" t="s">
+      <c r="B314" s="5" t="s">
         <v>1038</v>
       </c>
-      <c r="C314" s="3">
-        <v>2004.0</v>
-      </c>
-      <c r="D314" s="3" t="s">
+      <c r="C314" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D314" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="E314" s="3" t="s">
+      <c r="E314" s="5" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -9252,7 +9256,7 @@
       <c r="B315" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="C315" s="2" t="s">
+      <c r="C315" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D315" s="2" t="s">
@@ -9266,16 +9270,16 @@
       <c r="A316" s="1">
         <v>314.0</v>
       </c>
-      <c r="B316" s="3" t="s">
+      <c r="B316" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="C316" s="3">
-        <v>1973.0</v>
-      </c>
-      <c r="D316" s="3" t="s">
+      <c r="C316" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D316" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="E316" s="3" t="s">
+      <c r="E316" s="5" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -9286,7 +9290,7 @@
       <c r="B317" s="2" t="s">
         <v>1047</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="C317" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D317" s="2" t="s">
@@ -9303,7 +9307,7 @@
       <c r="B318" s="2" t="s">
         <v>1050</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="C318" s="3" t="s">
         <v>1051</v>
       </c>
       <c r="D318" s="2" t="s">
@@ -9320,7 +9324,7 @@
       <c r="B319" s="2" t="s">
         <v>1054</v>
       </c>
-      <c r="C319" s="2" t="s">
+      <c r="C319" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D319" s="2" t="s">
@@ -9337,7 +9341,7 @@
       <c r="B320" s="2" t="s">
         <v>1057</v>
       </c>
-      <c r="C320" s="2" t="s">
+      <c r="C320" s="3" t="s">
         <v>720</v>
       </c>
       <c r="D320" s="2" t="s">
@@ -9351,16 +9355,16 @@
       <c r="A321" s="1">
         <v>319.0</v>
       </c>
-      <c r="B321" s="3" t="s">
+      <c r="B321" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="C321" s="3">
-        <v>1982.0</v>
-      </c>
-      <c r="D321" s="3" t="s">
+      <c r="C321" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="D321" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="E321" s="3" t="s">
+      <c r="E321" s="5" t="s">
         <v>1062</v>
       </c>
     </row>
@@ -9371,7 +9375,7 @@
       <c r="B322" s="2" t="s">
         <v>1063</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="C322" s="3" t="s">
         <v>1064</v>
       </c>
       <c r="D322" s="2" t="s">
@@ -9385,16 +9389,16 @@
       <c r="A323" s="1">
         <v>321.0</v>
       </c>
-      <c r="B323" s="3" t="s">
+      <c r="B323" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="C323" s="3">
-        <v>1963.0</v>
-      </c>
-      <c r="D323" s="3" t="s">
+      <c r="C323" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="D323" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="E323" s="3" t="s">
+      <c r="E323" s="5" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -9405,7 +9409,7 @@
       <c r="B324" s="2" t="s">
         <v>1070</v>
       </c>
-      <c r="C324" s="2" t="s">
+      <c r="C324" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D324" s="2" t="s">
@@ -9422,7 +9426,7 @@
       <c r="B325" s="2" t="s">
         <v>1073</v>
       </c>
-      <c r="C325" s="2" t="s">
+      <c r="C325" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D325" s="2" t="s">
@@ -9439,7 +9443,7 @@
       <c r="B326" s="2" t="s">
         <v>1076</v>
       </c>
-      <c r="C326" s="2" t="s">
+      <c r="C326" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D326" s="2" t="s">
@@ -9456,7 +9460,7 @@
       <c r="B327" s="2" t="s">
         <v>1079</v>
       </c>
-      <c r="C327" s="2" t="s">
+      <c r="C327" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D327" s="2" t="s">
@@ -9473,7 +9477,7 @@
       <c r="B328" s="2" t="s">
         <v>1082</v>
       </c>
-      <c r="C328" s="2" t="s">
+      <c r="C328" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D328" s="2" t="s">
@@ -9490,7 +9494,7 @@
       <c r="B329" s="2" t="s">
         <v>1085</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="C329" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D329" s="2" t="s">
@@ -9507,7 +9511,7 @@
       <c r="B330" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="C330" s="2" t="s">
+      <c r="C330" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D330" s="2" t="s">
@@ -9521,16 +9525,16 @@
       <c r="A331" s="1">
         <v>329.0</v>
       </c>
-      <c r="B331" s="3" t="s">
+      <c r="B331" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="C331" s="3">
-        <v>1996.0</v>
-      </c>
-      <c r="D331" s="3" t="s">
+      <c r="C331" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D331" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="E331" s="3" t="s">
+      <c r="E331" s="5" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -9541,7 +9545,7 @@
       <c r="B332" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="C332" s="2" t="s">
+      <c r="C332" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D332" s="2" t="s">
@@ -9558,7 +9562,7 @@
       <c r="B333" s="2" t="s">
         <v>1097</v>
       </c>
-      <c r="C333" s="2" t="s">
+      <c r="C333" s="3" t="s">
         <v>615</v>
       </c>
       <c r="D333" s="2" t="s">
@@ -9575,7 +9579,7 @@
       <c r="B334" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="C334" s="2" t="s">
+      <c r="C334" s="3" t="s">
         <v>605</v>
       </c>
       <c r="D334" s="2" t="s">
@@ -9592,7 +9596,7 @@
       <c r="B335" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="C335" s="2" t="s">
+      <c r="C335" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D335" s="2" t="s">
@@ -9609,7 +9613,7 @@
       <c r="B336" s="2" t="s">
         <v>1013</v>
       </c>
-      <c r="C336" s="2" t="s">
+      <c r="C336" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D336" s="2" t="s">
@@ -9626,7 +9630,7 @@
       <c r="B337" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="C337" s="2" t="s">
+      <c r="C337" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D337" s="2" t="s">
@@ -9643,7 +9647,7 @@
       <c r="B338" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="C338" s="2" t="s">
+      <c r="C338" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D338" s="2" t="s">
@@ -9660,7 +9664,7 @@
       <c r="B339" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="C339" s="2" t="s">
+      <c r="C339" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D339" s="2" t="s">
@@ -9677,7 +9681,7 @@
       <c r="B340" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="C340" s="2" t="s">
+      <c r="C340" s="3" t="s">
         <v>626</v>
       </c>
       <c r="D340" s="2" t="s">
@@ -9694,7 +9698,7 @@
       <c r="B341" s="2" t="s">
         <v>1120</v>
       </c>
-      <c r="C341" s="2" t="s">
+      <c r="C341" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D341" s="2" t="s">
@@ -9711,7 +9715,7 @@
       <c r="B342" s="2" t="s">
         <v>1123</v>
       </c>
-      <c r="C342" s="2" t="s">
+      <c r="C342" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D342" s="2" t="s">
@@ -9728,7 +9732,7 @@
       <c r="B343" s="2" t="s">
         <v>1126</v>
       </c>
-      <c r="C343" s="2" t="s">
+      <c r="C343" s="3" t="s">
         <v>675</v>
       </c>
       <c r="D343" s="2" t="s">
@@ -9745,8 +9749,8 @@
       <c r="B344" s="2" t="s">
         <v>1129</v>
       </c>
-      <c r="C344" s="2" t="s">
-        <v>504</v>
+      <c r="C344" s="3" t="s">
+        <v>505</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>1130</v>
@@ -9762,13 +9766,13 @@
       <c r="B345" s="2" t="s">
         <v>1132</v>
       </c>
-      <c r="C345" s="2" t="s">
+      <c r="C345" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="D345" s="3" t="s">
+      <c r="D345" s="5" t="s">
         <v>1133</v>
       </c>
-      <c r="E345" s="3" t="s">
+      <c r="E345" s="5" t="s">
         <v>1134</v>
       </c>
     </row>
@@ -9779,7 +9783,7 @@
       <c r="B346" s="2" t="s">
         <v>1135</v>
       </c>
-      <c r="C346" s="2" t="s">
+      <c r="C346" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D346" s="2" t="s">
@@ -9796,7 +9800,7 @@
       <c r="B347" s="2" t="s">
         <v>1138</v>
       </c>
-      <c r="C347" s="2" t="s">
+      <c r="C347" s="3" t="s">
         <v>481</v>
       </c>
       <c r="D347" s="2" t="s">
@@ -9813,7 +9817,7 @@
       <c r="B348" s="2" t="s">
         <v>1141</v>
       </c>
-      <c r="C348" s="2" t="s">
+      <c r="C348" s="3" t="s">
         <v>652</v>
       </c>
       <c r="D348" s="2" t="s">
@@ -9830,7 +9834,7 @@
       <c r="B349" s="2" t="s">
         <v>1144</v>
       </c>
-      <c r="C349" s="2" t="s">
+      <c r="C349" s="3" t="s">
         <v>1145</v>
       </c>
       <c r="D349" s="2" t="s">
@@ -9847,7 +9851,7 @@
       <c r="B350" s="2" t="s">
         <v>1148</v>
       </c>
-      <c r="C350" s="2" t="s">
+      <c r="C350" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D350" s="2" t="s">
@@ -9864,7 +9868,7 @@
       <c r="B351" s="2" t="s">
         <v>1151</v>
       </c>
-      <c r="C351" s="2" t="s">
+      <c r="C351" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D351" s="2" t="s">
@@ -9881,8 +9885,8 @@
       <c r="B352" s="2" t="s">
         <v>1154</v>
       </c>
-      <c r="C352" s="2" t="s">
-        <v>567</v>
+      <c r="C352" s="3" t="s">
+        <v>488</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>1155</v>
@@ -9898,7 +9902,7 @@
       <c r="B353" s="2" t="s">
         <v>1157</v>
       </c>
-      <c r="C353" s="2" t="s">
+      <c r="C353" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D353" s="2" t="s">
@@ -9915,7 +9919,7 @@
       <c r="B354" s="2" t="s">
         <v>1160</v>
       </c>
-      <c r="C354" s="2" t="s">
+      <c r="C354" s="3" t="s">
         <v>601</v>
       </c>
       <c r="D354" s="2" t="s">
@@ -9932,7 +9936,7 @@
       <c r="B355" s="2" t="s">
         <v>1163</v>
       </c>
-      <c r="C355" s="2" t="s">
+      <c r="C355" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D355" s="2" t="s">
@@ -9949,7 +9953,7 @@
       <c r="B356" s="2" t="s">
         <v>1166</v>
       </c>
-      <c r="C356" s="2" t="s">
+      <c r="C356" s="3" t="s">
         <v>1167</v>
       </c>
       <c r="D356" s="2" t="s">
@@ -9966,7 +9970,7 @@
       <c r="B357" s="2" t="s">
         <v>1170</v>
       </c>
-      <c r="C357" s="2" t="s">
+      <c r="C357" s="3" t="s">
         <v>1171</v>
       </c>
       <c r="D357" s="2" t="s">
@@ -9980,16 +9984,16 @@
       <c r="A358" s="1">
         <v>356.0</v>
       </c>
-      <c r="B358" s="3" t="s">
+      <c r="B358" s="5" t="s">
         <v>1174</v>
       </c>
-      <c r="C358" s="3">
-        <v>1968.0</v>
-      </c>
-      <c r="D358" s="3" t="s">
+      <c r="C358" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D358" s="5" t="s">
         <v>1175</v>
       </c>
-      <c r="E358" s="3" t="s">
+      <c r="E358" s="5" t="s">
         <v>1176</v>
       </c>
     </row>
@@ -10000,7 +10004,7 @@
       <c r="B359" s="2" t="s">
         <v>1177</v>
       </c>
-      <c r="C359" s="2" t="s">
+      <c r="C359" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D359" s="2" t="s">
@@ -10017,8 +10021,8 @@
       <c r="B360" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="C360" s="2" t="s">
-        <v>504</v>
+      <c r="C360" s="3" t="s">
+        <v>505</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>1181</v>
@@ -10034,8 +10038,8 @@
       <c r="B361" s="2" t="s">
         <v>1183</v>
       </c>
-      <c r="C361" s="2" t="s">
-        <v>881</v>
+      <c r="C361" s="3" t="s">
+        <v>775</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>1184</v>
@@ -10051,7 +10055,7 @@
       <c r="B362" s="2" t="s">
         <v>1186</v>
       </c>
-      <c r="C362" s="2" t="s">
+      <c r="C362" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D362" s="2" t="s">
@@ -10068,7 +10072,7 @@
       <c r="B363" s="2" t="s">
         <v>1189</v>
       </c>
-      <c r="C363" s="2" t="s">
+      <c r="C363" s="3" t="s">
         <v>1035</v>
       </c>
       <c r="D363" s="2" t="s">
@@ -10085,7 +10089,7 @@
       <c r="B364" s="2" t="s">
         <v>1192</v>
       </c>
-      <c r="C364" s="2" t="s">
+      <c r="C364" s="3" t="s">
         <v>1193</v>
       </c>
       <c r="D364" s="2" t="s">
@@ -10102,7 +10106,7 @@
       <c r="B365" s="2" t="s">
         <v>1196</v>
       </c>
-      <c r="C365" s="2" t="s">
+      <c r="C365" s="3" t="s">
         <v>1197</v>
       </c>
       <c r="D365" s="2" t="s">
@@ -10119,7 +10123,7 @@
       <c r="B366" s="2" t="s">
         <v>1200</v>
       </c>
-      <c r="C366" s="2" t="s">
+      <c r="C366" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D366" s="2" t="s">

</xml_diff>